<commit_message>
New version of the block schedule
</commit_message>
<xml_diff>
--- a/assets/schedule/frontier.xlsx
+++ b/assets/schedule/frontier.xlsx
@@ -21,7 +21,7 @@
     <sheet name="Key!!" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="current_date">"2022-05-18 17:37:21.732107"</definedName>
+    <definedName name="current_date">"2022-05-20 00:50:47.845288"</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="L71" s="17" t="inlineStr">
         <is>
-          <t>NF All frontier (18N) (KNE 130 - 300 ppl)</t>
+          <t>NF All-Frontier (18N) (KNE 130 - 300 ppl)</t>
         </is>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
       </c>
       <c r="J101" s="17" t="inlineStr">
         <is>
-          <t>NF DUNE P5 Detector technology (20N) (KNE 120 - 150 ppl)</t>
+          <t>NF DUNE P5 Strategy (Detector Technology) (20N) (KNE 120 - 150 ppl)</t>
         </is>
       </c>
       <c r="K101" s="19" t="inlineStr">
@@ -2179,7 +2179,7 @@
       <c r="I104" s="9" t="n"/>
       <c r="J104" s="9" t="n"/>
       <c r="K104" s="9" t="n"/>
-      <c r="L104" t="inlineStr"/>
+      <c r="L104" s="9" t="n"/>
       <c r="M104" s="9" t="n"/>
       <c r="N104" s="9" t="n"/>
     </row>
@@ -2206,7 +2206,7 @@
       <c r="I105" s="9" t="n"/>
       <c r="J105" s="17" t="inlineStr">
         <is>
-          <t>NF DUNE P5 Expanded Phys Scope (20X) (KNE 110 - 150 ppl)</t>
+          <t>NF DUNE P5 Strategy (Expanded Physics Scope in Phase II) (20X) (KNE 110 - 150 ppl)</t>
         </is>
       </c>
       <c r="K105" s="19" t="inlineStr">
@@ -2279,7 +2279,7 @@
       <c r="I108" s="9" t="n"/>
       <c r="J108" s="9" t="n"/>
       <c r="K108" s="9" t="n"/>
-      <c r="L108" t="inlineStr"/>
+      <c r="L108" s="9" t="n"/>
       <c r="M108" s="9" t="n"/>
       <c r="N108" s="9" t="n"/>
     </row>
@@ -2680,7 +2680,6 @@
       <c r="N128" t="inlineStr"/>
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="inlineStr"/>
-      <c r="Q128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="B129" t="inlineStr">
@@ -2702,7 +2701,6 @@
       <c r="N129" t="inlineStr"/>
       <c r="O129" t="inlineStr"/>
       <c r="P129" t="inlineStr"/>
-      <c r="Q129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="B130" t="inlineStr">
@@ -2724,7 +2722,6 @@
       <c r="N130" t="inlineStr"/>
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="B131" t="inlineStr">
@@ -2784,7 +2781,7 @@
       </c>
       <c r="M131" s="17" t="inlineStr">
         <is>
-          <t>NF DUNE P5 oscillation physics (20O) (JHN 102 - 150 ppl)</t>
+          <t>NF DUNE P5 Strategy (Oscillation Physics) (20O) (JHN 102 - 150 ppl)</t>
         </is>
       </c>
       <c r="N131" s="19" t="inlineStr">
@@ -2802,7 +2799,6 @@
           <t>UF UF1 (18B) (25 ppl)</t>
         </is>
       </c>
-      <c r="Q131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="B132" t="inlineStr">
@@ -2824,7 +2820,6 @@
       <c r="N132" s="9" t="n"/>
       <c r="O132" s="9" t="n"/>
       <c r="P132" s="9" t="n"/>
-      <c r="Q132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="B133" t="inlineStr">
@@ -2846,7 +2841,6 @@
       <c r="N133" s="9" t="n"/>
       <c r="O133" s="9" t="n"/>
       <c r="P133" s="9" t="n"/>
-      <c r="Q133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="B134" t="inlineStr">
@@ -2867,12 +2861,7 @@
       <c r="M134" s="9" t="n"/>
       <c r="N134" s="9" t="n"/>
       <c r="O134" s="9" t="n"/>
-      <c r="P134" s="8" t="inlineStr">
-        <is>
-          <t>XF UF-NF Long Baseline (18Q) (40 ppl)</t>
-        </is>
-      </c>
-      <c r="Q134" t="inlineStr"/>
+      <c r="P134" s="9" t="n"/>
     </row>
     <row r="135">
       <c r="B135" t="inlineStr">
@@ -2896,7 +2885,7 @@
       <c r="L135" s="9" t="n"/>
       <c r="M135" s="17" t="inlineStr">
         <is>
-          <t>NF DUNE P5 BSM (20Y) (JHN 102 - 150 ppl)</t>
+          <t>NF DUNE P5 Strategy (BSM Physics) (20Y) (JHN 102 - 150 ppl)</t>
         </is>
       </c>
       <c r="N135" s="19" t="inlineStr">
@@ -2905,10 +2894,9 @@
         </is>
       </c>
       <c r="O135" s="9" t="n"/>
-      <c r="P135" s="9" t="n"/>
-      <c r="Q135" s="10" t="inlineStr">
-        <is>
-          <t>XF UF-IF QIS (22F) (HUB 214 - 50 ppl)</t>
+      <c r="P135" s="8" t="inlineStr">
+        <is>
+          <t>XF UF-NF Long Baseline (18Q) (40 ppl)</t>
         </is>
       </c>
     </row>
@@ -2932,7 +2920,6 @@
       <c r="N136" s="9" t="n"/>
       <c r="O136" s="9" t="n"/>
       <c r="P136" s="9" t="n"/>
-      <c r="Q136" s="9" t="n"/>
     </row>
     <row r="137">
       <c r="B137" t="inlineStr">
@@ -2953,8 +2940,7 @@
       <c r="M137" s="9" t="n"/>
       <c r="N137" s="9" t="n"/>
       <c r="O137" s="9" t="n"/>
-      <c r="P137" t="inlineStr"/>
-      <c r="Q137" s="9" t="n"/>
+      <c r="P137" s="9" t="n"/>
     </row>
     <row r="138">
       <c r="B138" t="inlineStr">
@@ -2975,8 +2961,7 @@
       <c r="M138" s="9" t="n"/>
       <c r="N138" s="9" t="n"/>
       <c r="O138" s="9" t="n"/>
-      <c r="P138" t="inlineStr"/>
-      <c r="Q138" s="9" t="n"/>
+      <c r="P138" s="9" t="n"/>
     </row>
     <row r="139">
       <c r="B139" t="inlineStr">
@@ -3002,7 +2987,6 @@
       <c r="N139" t="inlineStr"/>
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="inlineStr"/>
-      <c r="Q139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="B140" t="inlineStr">
@@ -3024,7 +3008,6 @@
       <c r="N140" t="inlineStr"/>
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="inlineStr"/>
-      <c r="Q140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="B141" t="inlineStr">
@@ -3046,7 +3029,6 @@
       <c r="N141" t="inlineStr"/>
       <c r="O141" t="inlineStr"/>
       <c r="P141" t="inlineStr"/>
-      <c r="Q141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="B142" t="inlineStr">
@@ -3068,7 +3050,6 @@
       <c r="N142" t="inlineStr"/>
       <c r="O142" t="inlineStr"/>
       <c r="P142" t="inlineStr"/>
-      <c r="Q142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="B143" t="inlineStr">
@@ -3098,7 +3079,6 @@
       <c r="N143" t="inlineStr"/>
       <c r="O143" t="inlineStr"/>
       <c r="P143" t="inlineStr"/>
-      <c r="Q143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="B144" t="inlineStr">
@@ -3120,7 +3100,6 @@
       <c r="N144" t="inlineStr"/>
       <c r="O144" t="inlineStr"/>
       <c r="P144" t="inlineStr"/>
-      <c r="Q144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="B145" t="inlineStr">
@@ -3142,7 +3121,6 @@
       <c r="N145" t="inlineStr"/>
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="inlineStr"/>
-      <c r="Q145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="B146" t="inlineStr">
@@ -3168,7 +3146,6 @@
       <c r="N146" t="inlineStr"/>
       <c r="O146" t="inlineStr"/>
       <c r="P146" t="inlineStr"/>
-      <c r="Q146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="B147" t="inlineStr">
@@ -3190,7 +3167,6 @@
       <c r="N147" t="inlineStr"/>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr"/>
-      <c r="Q147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="B148" t="inlineStr">
@@ -3212,7 +3188,6 @@
       <c r="N148" t="inlineStr"/>
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr"/>
-      <c r="Q148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="B149" t="inlineStr">
@@ -3234,7 +3209,6 @@
       <c r="N149" t="inlineStr"/>
       <c r="O149" t="inlineStr"/>
       <c r="P149" t="inlineStr"/>
-      <c r="Q149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="B150" t="inlineStr">
@@ -3256,7 +3230,6 @@
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr"/>
       <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="B151" t="inlineStr">
@@ -3278,7 +3251,6 @@
       <c r="N151" t="inlineStr"/>
       <c r="O151" t="inlineStr"/>
       <c r="P151" t="inlineStr"/>
-      <c r="Q151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="B152" t="inlineStr">
@@ -3300,7 +3272,6 @@
       <c r="N152" t="inlineStr"/>
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr"/>
-      <c r="Q152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="B153" t="inlineStr">
@@ -3322,7 +3293,6 @@
       <c r="N153" t="inlineStr"/>
       <c r="O153" t="inlineStr"/>
       <c r="P153" t="inlineStr"/>
-      <c r="Q153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="B154" t="inlineStr">
@@ -3348,7 +3318,6 @@
       <c r="N154" t="inlineStr"/>
       <c r="O154" t="inlineStr"/>
       <c r="P154" t="inlineStr"/>
-      <c r="Q154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="B155" t="inlineStr">
@@ -3370,7 +3339,6 @@
       <c r="N155" t="inlineStr"/>
       <c r="O155" t="inlineStr"/>
       <c r="P155" t="inlineStr"/>
-      <c r="Q155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="B156" t="inlineStr">
@@ -3392,7 +3360,6 @@
       <c r="N156" t="inlineStr"/>
       <c r="O156" t="inlineStr"/>
       <c r="P156" t="inlineStr"/>
-      <c r="Q156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="B157" t="inlineStr">
@@ -3414,7 +3381,6 @@
       <c r="N157" t="inlineStr"/>
       <c r="O157" t="inlineStr"/>
       <c r="P157" t="inlineStr"/>
-      <c r="Q157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="B158" t="inlineStr">
@@ -3522,7 +3488,7 @@
       </c>
       <c r="J161" s="24" t="inlineStr">
         <is>
-          <t>NF Beyond Neutrino Mass of precision beta-decay (21K) (20 ppl)</t>
+          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K) (20 ppl)</t>
         </is>
       </c>
       <c r="K161" s="24" t="inlineStr">
@@ -3532,7 +3498,7 @@
       </c>
       <c r="L161" s="22" t="inlineStr">
         <is>
-          <t>TF TF5-TF10 (18D) (JHN 111 - 50 ppl)</t>
+          <t>TF TF2-TF5 (18D) (JHN 111 - 50 ppl)</t>
         </is>
       </c>
       <c r="M161" s="8" t="inlineStr">
@@ -3550,7 +3516,11 @@
           <t>XF RF-EF-TF RF1 Flavor anomalies and exotics at colliders (22A) (HUB 340 - 50 ppl)</t>
         </is>
       </c>
-      <c r="P161" t="inlineStr"/>
+      <c r="P161" s="10" t="inlineStr">
+        <is>
+          <t>XF UF-IF QIS (22F) (HUB 337 - 50 ppl)</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="B162" t="inlineStr">
@@ -3571,7 +3541,7 @@
       <c r="M162" s="9" t="n"/>
       <c r="N162" s="9" t="n"/>
       <c r="O162" s="9" t="n"/>
-      <c r="P162" t="inlineStr"/>
+      <c r="P162" s="9" t="n"/>
     </row>
     <row r="163">
       <c r="B163" t="inlineStr">
@@ -3592,7 +3562,7 @@
       <c r="M163" s="9" t="n"/>
       <c r="N163" s="9" t="n"/>
       <c r="O163" s="9" t="n"/>
-      <c r="P163" t="inlineStr"/>
+      <c r="P163" s="9" t="n"/>
     </row>
     <row r="164">
       <c r="B164" t="inlineStr">
@@ -3613,7 +3583,7 @@
       <c r="M164" s="9" t="n"/>
       <c r="N164" s="9" t="n"/>
       <c r="O164" s="9" t="n"/>
-      <c r="P164" t="inlineStr"/>
+      <c r="P164" s="9" t="n"/>
     </row>
     <row r="165">
       <c r="B165" t="inlineStr">
@@ -4428,7 +4398,7 @@
       <c r="J197" s="9" t="n"/>
       <c r="K197" s="9" t="n"/>
       <c r="L197" s="9" t="n"/>
-      <c r="M197" t="inlineStr"/>
+      <c r="M197" s="9" t="n"/>
       <c r="N197" s="9" t="n"/>
       <c r="O197" s="9" t="n"/>
       <c r="P197" s="9" t="n"/>
@@ -4450,7 +4420,7 @@
       <c r="J198" s="9" t="n"/>
       <c r="K198" s="9" t="n"/>
       <c r="L198" s="9" t="n"/>
-      <c r="M198" t="inlineStr"/>
+      <c r="M198" s="9" t="n"/>
       <c r="N198" s="9" t="n"/>
       <c r="O198" s="9" t="n"/>
       <c r="P198" s="9" t="n"/>
@@ -4965,7 +4935,7 @@
       </c>
       <c r="C221" s="23" t="inlineStr">
         <is>
-          <t>AF All frontier (18M) (KNE 110 - 150 ppl)</t>
+          <t>AF All-Frontier (18M) (KNE 110 - 150 ppl)</t>
         </is>
       </c>
       <c r="D221" s="23" t="inlineStr">
@@ -4983,19 +4953,19 @@
           <t>IF Report (JHN 075 - 100 ppl)</t>
         </is>
       </c>
-      <c r="G221" s="17" t="inlineStr">
-        <is>
-          <t>NF Topical Group 1 (20K) (JHN 102 - 60 ppl)</t>
-        </is>
-      </c>
-      <c r="H221" s="24" t="inlineStr">
-        <is>
-          <t>NF Topical Group 3 (20I) (30 ppl)</t>
+      <c r="G221" s="24" t="inlineStr">
+        <is>
+          <t>NF Early Career Presentations (Topic 1) (20I) (30 ppl)</t>
+        </is>
+      </c>
+      <c r="H221" s="17" t="inlineStr">
+        <is>
+          <t>NF Early Career Presentations (Topic 2) (20K) (JHN 102 - 60 ppl)</t>
         </is>
       </c>
       <c r="I221" s="26" t="inlineStr">
         <is>
-          <t>RF All Frontier Discussions (23Y) (KNE 220 - 140 ppl)</t>
+          <t>RF All-Frontier Discussions (23Y) (KNE 220 - 140 ppl)</t>
         </is>
       </c>
       <c r="J221" s="27" t="inlineStr">
@@ -5005,7 +4975,7 @@
       </c>
       <c r="K221" s="22" t="inlineStr">
         <is>
-          <t>TF TF2-TF8 (18E) (JHN 111 - 50 ppl)</t>
+          <t>TF TF8-TF10 (18E) (JHN 111 - 50 ppl)</t>
         </is>
       </c>
       <c r="L221" s="8" t="inlineStr">
@@ -5767,7 +5737,7 @@
       </c>
       <c r="C255" s="23" t="inlineStr">
         <is>
-          <t>AF All frontier (KNE 120 - 150 ppl)</t>
+          <t>AF All-Frontier (KNE 120 - 150 ppl)</t>
         </is>
       </c>
       <c r="D255" s="12" t="inlineStr">
@@ -5780,19 +5750,19 @@
           <t>IF Report (24D) (JHN 102 - 100 ppl)</t>
         </is>
       </c>
-      <c r="F255" s="17" t="inlineStr">
-        <is>
-          <t>NF NF2 (20J) (JHN 175 - 60 ppl)</t>
+      <c r="F255" s="24" t="inlineStr">
+        <is>
+          <t>NF Community Engagement Success Stories (22I) (20 ppl)</t>
         </is>
       </c>
       <c r="G255" s="24" t="inlineStr">
         <is>
-          <t>NF NF4 (20H) (30 ppl)</t>
-        </is>
-      </c>
-      <c r="H255" s="24" t="inlineStr">
-        <is>
-          <t>NF Success stories from NF (22I) (20 ppl)</t>
+          <t>NF Early Career Presentations (Topic 3) (20H) (30 ppl)</t>
+        </is>
+      </c>
+      <c r="H255" s="17" t="inlineStr">
+        <is>
+          <t>NF Early Career Presentations (Topic 4) (20J) (JHN 175 - 60 ppl)</t>
         </is>
       </c>
       <c r="I255" s="22" t="inlineStr">
@@ -5891,7 +5861,7 @@
       <c r="G258" s="9" t="n"/>
       <c r="H258" s="9" t="n"/>
       <c r="I258" s="9" t="n"/>
-      <c r="J258" t="inlineStr"/>
+      <c r="J258" s="9" t="n"/>
       <c r="K258" s="9" t="n"/>
       <c r="L258" s="9" t="n"/>
       <c r="M258" s="9" t="n"/>
@@ -6858,7 +6828,7 @@
     <mergeCell ref="I101:I108"/>
     <mergeCell ref="J101:J104"/>
     <mergeCell ref="K101:K104"/>
-    <mergeCell ref="L101:L103"/>
+    <mergeCell ref="L101:L104"/>
     <mergeCell ref="M101:M108"/>
     <mergeCell ref="N101:N108"/>
     <mergeCell ref="F103:F104"/>
@@ -6866,7 +6836,7 @@
     <mergeCell ref="G105:G108"/>
     <mergeCell ref="J105:J108"/>
     <mergeCell ref="K105:K108"/>
-    <mergeCell ref="L105:L107"/>
+    <mergeCell ref="L105:L108"/>
     <mergeCell ref="F107:F108"/>
     <mergeCell ref="C109:C112"/>
     <mergeCell ref="C113:C115"/>
@@ -6885,12 +6855,11 @@
     <mergeCell ref="M131:M134"/>
     <mergeCell ref="N131:N134"/>
     <mergeCell ref="O131:O138"/>
-    <mergeCell ref="P131:P133"/>
-    <mergeCell ref="P134:P136"/>
+    <mergeCell ref="P131:P134"/>
     <mergeCell ref="F135:F138"/>
     <mergeCell ref="M135:M138"/>
     <mergeCell ref="N135:N138"/>
-    <mergeCell ref="Q135:Q138"/>
+    <mergeCell ref="P135:P138"/>
     <mergeCell ref="C139:C142"/>
     <mergeCell ref="C143:C145"/>
     <mergeCell ref="D143:D145"/>
@@ -6909,6 +6878,7 @@
     <mergeCell ref="M161:M164"/>
     <mergeCell ref="N161:N168"/>
     <mergeCell ref="O161:O164"/>
+    <mergeCell ref="P161:P164"/>
     <mergeCell ref="M165:M168"/>
     <mergeCell ref="O165:O168"/>
     <mergeCell ref="P165:P168"/>
@@ -6934,7 +6904,7 @@
     <mergeCell ref="Q191:Q194"/>
     <mergeCell ref="F195:F198"/>
     <mergeCell ref="L195:L198"/>
-    <mergeCell ref="M195:M196"/>
+    <mergeCell ref="M195:M198"/>
     <mergeCell ref="O195:O198"/>
     <mergeCell ref="P195:P198"/>
     <mergeCell ref="Q196:Q199"/>
@@ -6972,7 +6942,7 @@
     <mergeCell ref="G255:G258"/>
     <mergeCell ref="H255:H258"/>
     <mergeCell ref="I255:I258"/>
-    <mergeCell ref="J255:J257"/>
+    <mergeCell ref="J255:J258"/>
     <mergeCell ref="K255:K258"/>
     <mergeCell ref="L255:L258"/>
     <mergeCell ref="M255:M258"/>
@@ -7066,11 +7036,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>8am-9:30am</t>
+          <t>8am-10am</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="28" t="inlineStr">
         <is>
@@ -7097,11 +7067,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10am-11:30am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -7128,11 +7098,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8am-9:30am</t>
+          <t>8am-10am</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="28" t="inlineStr">
         <is>
@@ -7159,11 +7129,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9:30am-11am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="28" t="inlineStr">
         <is>
@@ -7185,12 +7155,12 @@
     <row r="8">
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>7-20</t>
+          <t>7-21</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10am-12pm</t>
+          <t>8am-10am</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -7198,11 +7168,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>HUB 214</t>
+          <t>HUB 337</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="G8" t="n">
         <v>50</v>
@@ -7221,11 +7191,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10am-11am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="28" t="inlineStr">
         <is>
@@ -7314,11 +7284,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>10am-11:30am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="28" t="inlineStr">
         <is>
@@ -8879,7 +8849,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>NF All frontier (18N)</t>
+          <t>NF All-Frontier (18N)</t>
         </is>
       </c>
     </row>
@@ -8910,7 +8880,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>NF DUNE P5 Detector technology (20N)</t>
+          <t>NF DUNE P5 Strategy (Detector Technology) (20N)</t>
         </is>
       </c>
     </row>
@@ -8922,11 +8892,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10am-11:30am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -8972,7 +8942,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>NF DUNE P5 Expanded Phys Scope (20X)</t>
+          <t>NF DUNE P5 Strategy (Expanded Physics Scope in Phase II) (20X)</t>
         </is>
       </c>
     </row>
@@ -9003,7 +8973,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>NF DUNE P5 oscillation physics (20O)</t>
+          <t>NF DUNE P5 Strategy (Oscillation Physics) (20O)</t>
         </is>
       </c>
     </row>
@@ -9015,11 +8985,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9:30am-11am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E9" s="28" t="inlineStr">
         <is>
@@ -9065,7 +9035,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>NF DUNE P5 BSM (20Y)</t>
+          <t>NF DUNE P5 Strategy (BSM Physics) (20Y)</t>
         </is>
       </c>
     </row>
@@ -9096,7 +9066,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>NF Beyond Neutrino Mass of precision beta-decay (21K)</t>
+          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K)</t>
         </is>
       </c>
     </row>
@@ -9220,7 +9190,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>NF Topical Group 3 (20I)</t>
+          <t>NF Early Career Presentations (Topic 1) (20I)</t>
         </is>
       </c>
     </row>
@@ -9313,7 +9283,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>NF Topical Group 1 (20K)</t>
+          <t>NF Early Career Presentations (Topic 2) (20K)</t>
         </is>
       </c>
     </row>
@@ -9375,7 +9345,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>NF Success stories from NF (22I)</t>
+          <t>NF Community Engagement Success Stories (22I)</t>
         </is>
       </c>
     </row>
@@ -9468,7 +9438,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>NF NF4 (20H)</t>
+          <t>NF Early Career Presentations (Topic 3) (20H)</t>
         </is>
       </c>
     </row>
@@ -9499,7 +9469,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>NF NF2 (20J)</t>
+          <t>NF Early Career Presentations (Topic 4) (20J)</t>
         </is>
       </c>
     </row>
@@ -9672,11 +9642,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>10am-11:30am</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -10032,7 +10002,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>RF All Frontier Discussions (23Y)</t>
+          <t>RF All-Frontier Discussions (23Y)</t>
         </is>
       </c>
     </row>
@@ -10943,7 +10913,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>TF TF5-TF10 (18D)</t>
+          <t>TF TF2-TF5 (18D)</t>
         </is>
       </c>
     </row>
@@ -11129,7 +11099,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>TF TF2-TF8 (18E)</t>
+          <t>TF TF8-TF10 (18E)</t>
         </is>
       </c>
     </row>
@@ -11817,7 +11787,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>AF All frontier (18M)</t>
+          <t>AF All-Frontier (18M)</t>
         </is>
       </c>
     </row>
@@ -11941,7 +11911,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>AF All frontier</t>
+          <t>AF All-Frontier</t>
         </is>
       </c>
     </row>
@@ -12233,31 +12203,31 @@
     <row r="11">
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>7-20</t>
+          <t>7-21</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10am-12pm</t>
+          <t>8am-12pm</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>HUB 214</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>80</v>
-      </c>
-      <c r="G11" t="n">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="E11" s="28" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F11" s="29" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="29" t="n">
+        <v>20</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>XF UF-IF QIS (22F)</t>
+          <t>IF IF7 (24G)</t>
         </is>
       </c>
     </row>
@@ -12284,11 +12254,11 @@
         <v>-1</v>
       </c>
       <c r="G12" s="29" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>IF IF7 (24G)</t>
+          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I)</t>
         </is>
       </c>
     </row>
@@ -12331,26 +12301,26 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>8am-12pm</t>
+          <t>8am-10am</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
-      </c>
-      <c r="E14" s="28" t="inlineStr">
-        <is>
-          <t>???</t>
-        </is>
-      </c>
-      <c r="F14" s="29" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G14" s="29" t="n">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>HUB 337</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" t="n">
+        <v>50</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I)</t>
+          <t>XF UF-IF QIS (22F)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update schedule (minor changes)
</commit_message>
<xml_diff>
--- a/assets/schedule/frontier.xlsx
+++ b/assets/schedule/frontier.xlsx
@@ -22,7 +22,7 @@
     <sheet name="Key!!" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="current_date">"2022-06-08 13:58:44.195639"</definedName>
+    <definedName name="current_date">"2022-06-13 17:57:03.179052"</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C39" s="10" t="inlineStr">
         <is>
-          <t>Registration (17REG) (KNE Lobby - 430 ppl)</t>
+          <t>Registration (17REG) (KNE Lobby - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="C42" s="10" t="inlineStr">
         <is>
-          <t>Introductory Plenary (17B) (KNE 130 - 430 ppl)</t>
+          <t>Introductory Plenary (17B) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="C48" s="11" t="inlineStr">
         <is>
-          <t>Lunch (17LUN) (430 ppl)</t>
+          <t>Lunch (17LUN) (476 ppl)</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C52" s="10" t="inlineStr">
         <is>
-          <t>Introductory Plenary (17D) (KNE 130 - 430 ppl)</t>
+          <t>Introductory Plenary (17D) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="C57" s="10" t="inlineStr">
         <is>
-          <t>Planning US HEP - past present future (17E) (KNE 130 - 430 ppl)</t>
+          <t>Planning US HEP - past present future (17E) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C77" s="11" t="inlineStr">
         <is>
-          <t>Lunch (18LUN) (430 ppl)</t>
+          <t>Lunch (18LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
@@ -1764,12 +1764,12 @@
       </c>
       <c r="C81" s="10" t="inlineStr">
         <is>
-          <t>AI/ML (172 ppl)</t>
+          <t>AI/ML (190 ppl)</t>
         </is>
       </c>
       <c r="D81" s="10" t="inlineStr">
         <is>
-          <t>Underground (18U) (KNE 130 - 129 ppl)</t>
+          <t>Underground (18U) (KNE 130 - 142 ppl)</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -1826,12 +1826,12 @@
       </c>
       <c r="C84" s="10" t="inlineStr">
         <is>
-          <t>Lattice QCD (86 ppl)</t>
+          <t>Lattice QCD (95 ppl)</t>
         </is>
       </c>
       <c r="D84" s="10" t="inlineStr">
         <is>
-          <t>The Next Accelerators (KNE 130 - 172 ppl)</t>
+          <t>The Next Accelerators (KNE 130 - 190 ppl)</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="C88" s="10" t="inlineStr">
         <is>
-          <t>DEI Talks and Panel (18Z) (KNE 130 - 215 ppl)</t>
+          <t>DEI Talks and Panel (18Z) (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="C106" s="11" t="inlineStr">
         <is>
-          <t>Lunch (19LUN) (430 ppl)</t>
+          <t>Lunch (19LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="C110" s="10" t="inlineStr">
         <is>
-          <t>Panel - Careers and Training the Next Generations (19S) (KNE 130 - 215 ppl)</t>
+          <t>Panel - Careers and Training the Next Generations (19S) (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D110" t="inlineStr"/>
@@ -2506,12 +2506,12 @@
       </c>
       <c r="C113" s="10" t="inlineStr">
         <is>
-          <t>Cosmic (172 ppl)</t>
+          <t>Cosmic (190 ppl)</t>
         </is>
       </c>
       <c r="D113" s="10" t="inlineStr">
         <is>
-          <t>Lepton Colliders (19S) (KNE 130 - 172 ppl)</t>
+          <t>Lepton Colliders (19S) (KNE 130 - 190 ppl)</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="C117" s="10" t="inlineStr">
         <is>
-          <t>Community Engagement (19V) (KNE 130 - 129 ppl)</t>
+          <t>Community Engagement (19V) (KNE 130 - 142 ppl)</t>
         </is>
       </c>
       <c r="D117" t="inlineStr"/>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="C135" s="11" t="inlineStr">
         <is>
-          <t>Lunch (20LUN) (430 ppl)</t>
+          <t>Lunch (20LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D135" t="inlineStr"/>
@@ -3106,12 +3106,12 @@
       </c>
       <c r="C139" s="10" t="inlineStr">
         <is>
-          <t>Neutrino (20BB) (KNE 130 - 172 ppl)</t>
+          <t>Neutrino (20BB) (KNE 130 - 190 ppl)</t>
         </is>
       </c>
       <c r="D139" s="10" t="inlineStr">
         <is>
-          <t>Rare Processes and AMO (215 ppl)</t>
+          <t>Rare Processes and AMO (238 ppl)</t>
         </is>
       </c>
       <c r="E139" t="inlineStr"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="C142" s="10" t="inlineStr">
         <is>
-          <t>Instrumentation (KNE 130 - 215 ppl)</t>
+          <t>Instrumentation (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
@@ -3473,32 +3473,32 @@
       </c>
       <c r="H156" s="27" t="inlineStr">
         <is>
-          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K) (20 ppl)</t>
-        </is>
-      </c>
-      <c r="I156" s="27" t="inlineStr">
-        <is>
           <t>NF Blue Skye/Very Long Term ideas (21M) (30 ppl)</t>
         </is>
       </c>
-      <c r="J156" s="25" t="inlineStr">
+      <c r="I156" s="25" t="inlineStr">
         <is>
           <t>TF TF2-TF5 (18D) (JHN 111 - 50 ppl)</t>
         </is>
       </c>
+      <c r="J156" s="26" t="inlineStr">
+        <is>
+          <t>XF EF-CompF EF Centric Discussions (18X) (40 ppl)</t>
+        </is>
+      </c>
       <c r="K156" s="26" t="inlineStr">
         <is>
-          <t>XF EF-CompF EF Centric Discussions (18X) (40 ppl)</t>
+          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I) (40 ppl)</t>
         </is>
       </c>
       <c r="L156" s="26" t="inlineStr">
         <is>
-          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I) (40 ppl)</t>
+          <t>XF IF-RF-EF Focus on timing and more generally tracking detectors (21J) (40 ppl)</t>
         </is>
       </c>
       <c r="M156" s="26" t="inlineStr">
         <is>
-          <t>XF IF-RF-EF Focus on timing and more generally tracking detectors (21J) (40 ppl)</t>
+          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C) (30 ppl)</t>
         </is>
       </c>
       <c r="N156" s="20" t="inlineStr">
@@ -3585,18 +3585,18 @@
       <c r="G160" s="9" t="n"/>
       <c r="H160" s="9" t="n"/>
       <c r="I160" s="9" t="n"/>
-      <c r="J160" s="9" t="n"/>
-      <c r="K160" s="15" t="inlineStr">
+      <c r="J160" s="15" t="inlineStr">
         <is>
           <t>CompF CompF7 Reinterpretation and long-term preservation of data and code (20D) (20 ppl)</t>
         </is>
       </c>
-      <c r="L160" s="9" t="n"/>
-      <c r="M160" s="16" t="inlineStr">
+      <c r="K160" s="9" t="n"/>
+      <c r="L160" s="16" t="inlineStr">
         <is>
           <t>EF DM Discussion (21N) (KNE 110 - 100 ppl)</t>
         </is>
       </c>
+      <c r="M160" s="9" t="n"/>
       <c r="N160" s="26" t="inlineStr">
         <is>
           <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B) (30 ppl)</t>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="C164" s="11" t="inlineStr">
         <is>
-          <t>Lunch (21LUN) (430 ppl)</t>
+          <t>Lunch (21LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D164" t="inlineStr"/>
@@ -3760,7 +3760,7 @@
       </c>
       <c r="C168" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Rare Processes and Precision Measurements (21U) (129 ppl)</t>
+          <t>Colloquium on Rare Processes and Precision Measurements (21U) (142 ppl)</t>
         </is>
       </c>
       <c r="D168" t="inlineStr"/>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="C171" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on New Accelerator and R&amp;D (129 ppl)</t>
+          <t>Colloquium on New Accelerator and R&amp;D (142 ppl)</t>
         </is>
       </c>
       <c r="D171" t="inlineStr"/>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="C175" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Cosmic Frontier Probes of Fundamental Physics (23W) (KNE 130 - 172 ppl)</t>
+          <t>Colloquium on Cosmic Frontier Probes of Fundamental Physics (23W) (KNE 130 - 190 ppl)</t>
         </is>
       </c>
       <c r="D175" t="inlineStr"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="C193" s="11" t="inlineStr">
         <is>
-          <t>Lunch (22LUN) (430 ppl)</t>
+          <t>Lunch (22LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D193" t="inlineStr"/>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="C197" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Underground Physics (22V) (KNE 130 - 129 ppl)</t>
+          <t>Colloquium on Underground Physics (22V) (KNE 130 - 142 ppl)</t>
         </is>
       </c>
       <c r="D197" t="inlineStr"/>
@@ -4492,7 +4492,7 @@
       </c>
       <c r="C200" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Theory (172 ppl)</t>
+          <t>Colloquium on Theory (190 ppl)</t>
         </is>
       </c>
       <c r="D200" t="inlineStr"/>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="C203" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Neutrino Physics (22W) (KNE 130 - 215 ppl)</t>
+          <t>Colloquium on Neutrino Physics (22W) (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D203" t="inlineStr"/>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="C222" s="11" t="inlineStr">
         <is>
-          <t>Lunch (23LUN) (430 ppl)</t>
+          <t>Lunch (23LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D222" t="inlineStr"/>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="C226" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Energy Frontier Physics (21W) (KNE 130 - 215 ppl)</t>
+          <t>Colloquium on Energy Frontier Physics (21W) (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D226" t="inlineStr"/>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="C229" s="10" t="inlineStr">
         <is>
-          <t>Colloquium on Computing (172 ppl)</t>
+          <t>Colloquium on Computing (190 ppl)</t>
         </is>
       </c>
       <c r="D229" t="inlineStr"/>
@@ -5262,7 +5262,7 @@
       </c>
       <c r="C233" s="10" t="inlineStr">
         <is>
-          <t>Quantum Information Science in HEP (23X) (KNE 130 - 215 ppl)</t>
+          <t>Quantum Information Science in HEP (23X) (KNE 130 - 238 ppl)</t>
         </is>
       </c>
       <c r="D233" t="inlineStr"/>
@@ -5575,42 +5575,42 @@
       </c>
       <c r="F247" s="27" t="inlineStr">
         <is>
+          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K) (20 ppl)</t>
+        </is>
+      </c>
+      <c r="G247" s="27" t="inlineStr">
+        <is>
           <t>NF Community Engagement Success Stories (22I) (20 ppl)</t>
         </is>
       </c>
-      <c r="G247" s="27" t="inlineStr">
+      <c r="H247" s="27" t="inlineStr">
         <is>
           <t>NF Early Career Presentations (Topic 3) (20H) (30 ppl)</t>
         </is>
       </c>
-      <c r="H247" s="19" t="inlineStr">
+      <c r="I247" s="19" t="inlineStr">
         <is>
           <t>NF Early Career Presentations (Topic 4) (20J) (JHN 175 - 60 ppl)</t>
         </is>
       </c>
-      <c r="I247" s="25" t="inlineStr">
+      <c r="J247" s="25" t="inlineStr">
         <is>
           <t>TF Discussion and frontier reports (19P) (KNE 220 - 175 ppl)</t>
         </is>
       </c>
-      <c r="J247" s="23" t="inlineStr">
+      <c r="K247" s="23" t="inlineStr">
         <is>
           <t>UF UF6 (23B) (25 ppl)</t>
         </is>
       </c>
-      <c r="K247" s="20" t="inlineStr">
+      <c r="L247" s="20" t="inlineStr">
         <is>
           <t>XF AF-CompF Cross-cutting issues (22E) (JHN 075 - 70 ppl)</t>
         </is>
       </c>
-      <c r="L247" s="26" t="inlineStr">
+      <c r="M247" s="26" t="inlineStr">
         <is>
           <t>XF AF-RF cross-cutting issues (22B) (40 ppl)</t>
-        </is>
-      </c>
-      <c r="M247" s="26" t="inlineStr">
-        <is>
-          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C) (30 ppl)</t>
         </is>
       </c>
       <c r="N247" s="20" t="inlineStr">
@@ -5700,7 +5700,7 @@
       </c>
       <c r="C251" s="11" t="inlineStr">
         <is>
-          <t>Lunch (24LUN) (430 ppl)</t>
+          <t>Lunch (24LUN) (476 ppl)</t>
         </is>
       </c>
       <c r="D251" t="inlineStr"/>
@@ -5788,7 +5788,7 @@
       </c>
       <c r="C255" s="10" t="inlineStr">
         <is>
-          <t>Snowmass Early Career (24S) (KNE 130 - 129 ppl)</t>
+          <t>Snowmass Early Career (24S) (KNE 130 - 142 ppl)</t>
         </is>
       </c>
       <c r="D255" t="inlineStr"/>
@@ -5855,12 +5855,12 @@
       </c>
       <c r="C258" s="10" t="inlineStr">
         <is>
-          <t>Instrumentation Projects (129 ppl)</t>
+          <t>Instrumentation Projects (142 ppl)</t>
         </is>
       </c>
       <c r="D258" s="10" t="inlineStr">
         <is>
-          <t>Underrepresented Minorities (KNE 130 - 129 ppl)</t>
+          <t>Underrepresented Minorities (KNE 130 - 142 ppl)</t>
         </is>
       </c>
       <c r="E258" t="inlineStr"/>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="C262" s="10" t="inlineStr">
         <is>
-          <t>DOE NSF FNAL Director and other US Labs Panel (24U) (KNE 130 - 258 ppl)</t>
+          <t>DOE NSF FNAL Director and other US Labs Panel (24U) (KNE 130 - 285 ppl)</t>
         </is>
       </c>
       <c r="D262" t="inlineStr"/>
@@ -6122,7 +6122,7 @@
       </c>
       <c r="C272" s="10" t="inlineStr">
         <is>
-          <t>Summary Plenary (25B) (KNE 130 - 430 ppl)</t>
+          <t>Summary Plenary (25B) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="C277" s="10" t="inlineStr">
         <is>
-          <t>Communicating HEP to the public and govt (KNE 130 - 430 ppl)</t>
+          <t>Communicating HEP to the public and govt (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="C280" s="11" t="inlineStr">
         <is>
-          <t>Lunch (25LUN) (430 ppl)</t>
+          <t>Lunch (25LUN) (476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="C284" s="10" t="inlineStr">
         <is>
-          <t>Panel - interconnections between frontiers and other fields panel (25C) (KNE 130 - 430 ppl)</t>
+          <t>Panel - interconnections between frontiers and other fields panel (25C) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="C288" s="10" t="inlineStr">
         <is>
-          <t>Talks - National International Leaders (KNE 130 - 430 ppl)</t>
+          <t>Talks - National International Leaders (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="C291" s="10" t="inlineStr">
         <is>
-          <t>Panel - International Status and Plans (KNE 130 - 430 ppl)</t>
+          <t>Panel - International Status and Plans (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6386,7 +6386,7 @@
       </c>
       <c r="C302" s="10" t="inlineStr">
         <is>
-          <t>Closeout Plenary (26B) (KNE 130 - 430 ppl)</t>
+          <t>Closeout Plenary (26B) (KNE 130 - 476 ppl)</t>
         </is>
       </c>
     </row>
@@ -6666,14 +6666,14 @@
     <mergeCell ref="G156:G163"/>
     <mergeCell ref="H156:H163"/>
     <mergeCell ref="I156:I163"/>
-    <mergeCell ref="J156:J163"/>
-    <mergeCell ref="K156:K159"/>
-    <mergeCell ref="L156:L163"/>
-    <mergeCell ref="M156:M159"/>
+    <mergeCell ref="J156:J159"/>
+    <mergeCell ref="K156:K163"/>
+    <mergeCell ref="L156:L159"/>
+    <mergeCell ref="M156:M163"/>
     <mergeCell ref="N156:N159"/>
     <mergeCell ref="O156:O159"/>
-    <mergeCell ref="K160:K163"/>
-    <mergeCell ref="M160:M163"/>
+    <mergeCell ref="J160:J163"/>
+    <mergeCell ref="L160:L163"/>
     <mergeCell ref="N160:N163"/>
     <mergeCell ref="O160:O163"/>
     <mergeCell ref="C164:C167"/>
@@ -9204,32 +9204,32 @@
       </c>
       <c r="H38" s="27" t="inlineStr">
         <is>
-          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K) (20 ppl)</t>
-        </is>
-      </c>
-      <c r="I38" s="27" t="inlineStr">
-        <is>
           <t>NF Blue Skye/Very Long Term ideas (21M) (30 ppl)</t>
         </is>
       </c>
-      <c r="J38" s="25" t="inlineStr">
+      <c r="I38" s="25" t="inlineStr">
         <is>
           <t>TF TF2-TF5 (18D) (JHN 111 - 50 ppl)</t>
         </is>
       </c>
+      <c r="J38" s="26" t="inlineStr">
+        <is>
+          <t>XF EF-CompF EF Centric Discussions (18X) (40 ppl)</t>
+        </is>
+      </c>
       <c r="K38" s="26" t="inlineStr">
         <is>
-          <t>XF EF-CompF EF Centric Discussions (18X) (40 ppl)</t>
+          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I) (40 ppl)</t>
         </is>
       </c>
       <c r="L38" s="26" t="inlineStr">
         <is>
-          <t>XF IF-EF-AF-IF Detectors and MDI and Plots (21I) (40 ppl)</t>
+          <t>XF IF-RF-EF Focus on timing and more generally tracking detectors (21J) (40 ppl)</t>
         </is>
       </c>
       <c r="M38" s="26" t="inlineStr">
         <is>
-          <t>XF IF-RF-EF Focus on timing and more generally tracking detectors (21J) (40 ppl)</t>
+          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C) (30 ppl)</t>
         </is>
       </c>
       <c r="N38" s="20" t="inlineStr">
@@ -9316,18 +9316,18 @@
       <c r="G42" s="9" t="n"/>
       <c r="H42" s="9" t="n"/>
       <c r="I42" s="9" t="n"/>
-      <c r="J42" s="9" t="n"/>
-      <c r="K42" s="15" t="inlineStr">
+      <c r="J42" s="15" t="inlineStr">
         <is>
           <t>CompF CompF7 Reinterpretation and long-term preservation of data and code (20D) (20 ppl)</t>
         </is>
       </c>
-      <c r="L42" s="9" t="n"/>
-      <c r="M42" s="16" t="inlineStr">
+      <c r="K42" s="9" t="n"/>
+      <c r="L42" s="16" t="inlineStr">
         <is>
           <t>EF DM Discussion (21N) (KNE 110 - 100 ppl)</t>
         </is>
       </c>
+      <c r="M42" s="9" t="n"/>
       <c r="N42" s="26" t="inlineStr">
         <is>
           <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B) (30 ppl)</t>
@@ -10097,42 +10097,42 @@
       </c>
       <c r="F72" s="27" t="inlineStr">
         <is>
+          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K) (20 ppl)</t>
+        </is>
+      </c>
+      <c r="G72" s="27" t="inlineStr">
+        <is>
           <t>NF Community Engagement Success Stories (22I) (20 ppl)</t>
         </is>
       </c>
-      <c r="G72" s="27" t="inlineStr">
+      <c r="H72" s="27" t="inlineStr">
         <is>
           <t>NF Early Career Presentations (Topic 3) (20H) (30 ppl)</t>
         </is>
       </c>
-      <c r="H72" s="19" t="inlineStr">
+      <c r="I72" s="19" t="inlineStr">
         <is>
           <t>NF Early Career Presentations (Topic 4) (20J) (JHN 175 - 60 ppl)</t>
         </is>
       </c>
-      <c r="I72" s="25" t="inlineStr">
+      <c r="J72" s="25" t="inlineStr">
         <is>
           <t>TF Discussion and frontier reports (19P) (KNE 220 - 175 ppl)</t>
         </is>
       </c>
-      <c r="J72" s="23" t="inlineStr">
+      <c r="K72" s="23" t="inlineStr">
         <is>
           <t>UF UF6 (23B) (25 ppl)</t>
         </is>
       </c>
-      <c r="K72" s="20" t="inlineStr">
+      <c r="L72" s="20" t="inlineStr">
         <is>
           <t>XF AF-CompF Cross-cutting issues (22E) (JHN 075 - 70 ppl)</t>
         </is>
       </c>
-      <c r="L72" s="26" t="inlineStr">
+      <c r="M72" s="26" t="inlineStr">
         <is>
           <t>XF AF-RF cross-cutting issues (22B) (40 ppl)</t>
-        </is>
-      </c>
-      <c r="M72" s="26" t="inlineStr">
-        <is>
-          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C) (30 ppl)</t>
         </is>
       </c>
       <c r="N72" s="20" t="inlineStr">
@@ -10297,14 +10297,14 @@
     <mergeCell ref="G38:G45"/>
     <mergeCell ref="H38:H45"/>
     <mergeCell ref="I38:I45"/>
-    <mergeCell ref="J38:J45"/>
-    <mergeCell ref="K38:K41"/>
-    <mergeCell ref="L38:L45"/>
-    <mergeCell ref="M38:M41"/>
+    <mergeCell ref="J38:J41"/>
+    <mergeCell ref="K38:K45"/>
+    <mergeCell ref="L38:L41"/>
+    <mergeCell ref="M38:M45"/>
     <mergeCell ref="N38:N41"/>
     <mergeCell ref="O38:O41"/>
-    <mergeCell ref="K42:K45"/>
-    <mergeCell ref="M42:M45"/>
+    <mergeCell ref="J42:J45"/>
+    <mergeCell ref="L42:L45"/>
     <mergeCell ref="N42:N45"/>
     <mergeCell ref="O42:O45"/>
     <mergeCell ref="C48:C55"/>
@@ -11444,11 +11444,11 @@
         <v>-1</v>
       </c>
       <c r="G12" s="32" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K)</t>
+          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C)</t>
         </is>
       </c>
     </row>
@@ -11785,11 +11785,11 @@
         <v>-1</v>
       </c>
       <c r="G23" s="32" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C)</t>
+          <t>NF Beyond neutrino mass physics reach of precision beta-decay experiments (21K)</t>
         </is>
       </c>
     </row>
@@ -12997,20 +12997,20 @@
       <c r="D15" t="n">
         <v>4</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>KNE 120</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>435</v>
-      </c>
-      <c r="G15" t="n">
-        <v>200</v>
+      <c r="E15" s="31" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F15" s="32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="32" t="n">
+        <v>30</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>CF Report Discussion (24M)</t>
+          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C)</t>
         </is>
       </c>
     </row>
@@ -13022,42 +13022,42 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10am-12pm</t>
+          <t>8am-12pm</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="31" t="inlineStr">
-        <is>
-          <t>???</t>
-        </is>
-      </c>
-      <c r="F16" s="32" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="32" t="n">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>KNE 120</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>435</v>
+      </c>
+      <c r="G16" t="n">
+        <v>200</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B)</t>
+          <t>CF Report Discussion (24M)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>7-23</t>
+          <t>7-21</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8am-12pm</t>
+          <t>10am-12pm</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="31" t="inlineStr">
         <is>
@@ -13072,7 +13072,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>XF IF-CF-CompF Instrumentation for Cosmic Frontier (21H)</t>
+          <t>XF RF-CF RF1 large-volume data analysis and simulation and usage of HPC in data analysis (24B)</t>
         </is>
       </c>
     </row>
@@ -13090,20 +13090,20 @@
       <c r="D18" t="n">
         <v>4</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>KNE 210</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>242</v>
-      </c>
-      <c r="G18" t="n">
-        <v>50</v>
+      <c r="E18" s="31" t="inlineStr">
+        <is>
+          <t>???</t>
+        </is>
+      </c>
+      <c r="F18" s="32" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="32" t="n">
+        <v>30</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>XF NF-CF-IF Dark matter detector (22J)</t>
+          <t>XF IF-CF-CompF Instrumentation for Cosmic Frontier (21H)</t>
         </is>
       </c>
     </row>
@@ -13123,49 +13123,49 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>KNE 120</t>
+          <t>KNE 210</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>435</v>
+        <v>242</v>
       </c>
       <c r="G19" t="n">
         <v>50</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>XF TF-CF Cosmic Frontier Theory (19K)</t>
+          <t>XF NF-CF-IF Dark matter detector (22J)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>7-24</t>
+          <t>7-23</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>10am-12pm</t>
+          <t>8am-12pm</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
-      </c>
-      <c r="E20" s="31" t="inlineStr">
-        <is>
-          <t>???</t>
-        </is>
-      </c>
-      <c r="F20" s="32" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G20" s="32" t="n">
-        <v>30</v>
+        <v>4</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>KNE 120</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>435</v>
+      </c>
+      <c r="G20" t="n">
+        <v>50</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>XF NF-CF Neutrino mass scale with beta decay kinematics (22C)</t>
+          <t>XF TF-CF Cosmic Frontier Theory (19K)</t>
         </is>
       </c>
     </row>

</xml_diff>